<commit_message>
Update Facebook login test cases.xlsx
</commit_message>
<xml_diff>
--- a/Facebook login test cases.xlsx
+++ b/Facebook login test cases.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mraje\learning\testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mraje\Documents\GitHub\QA-presentations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA379363-1F0F-4DFA-9F1B-CBDA329258D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B7E0882-CFC9-4095-A51B-8EA3523DE5EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="3" xr2:uid="{B7BD01C3-DC10-45CD-9FAD-FF36DF8655F5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{B7BD01C3-DC10-45CD-9FAD-FF36DF8655F5}"/>
   </bookViews>
   <sheets>
     <sheet name="Scenarios " sheetId="2" r:id="rId1"/>
@@ -563,7 +563,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -590,6 +590,9 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -909,8 +912,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44BBC577-987C-4641-B6C4-456753410AFC}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -921,17 +924,17 @@
     <col min="5" max="16384" width="8.88671875" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="10" t="s">
         <v>107</v>
       </c>
     </row>
@@ -1541,7 +1544,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B632A1D8-013B-45DD-83B4-982F316E0B7C}">
   <dimension ref="A1:M12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+    <sheetView topLeftCell="A11" workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>

</xml_diff>